<commit_message>
major changes for data
</commit_message>
<xml_diff>
--- a/ipa_2/myUtils/ecologicals_A.xlsx
+++ b/ipa_2/myUtils/ecologicals_A.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomer\Documents\GitHub\WebExperiment\ipa_1_2\myUtils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomer\Documents\GitHub\WebExperiment\ipa_2\myUtils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEEAE2C-FB03-4334-BE4D-69BDDA005CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E41B2E1-E809-4246-B519-EDD1C804B4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3732" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -98,16 +98,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="A6" sqref="A6:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -401,287 +397,159 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="J1" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>992179</v>
+        <v>99881</v>
       </c>
       <c r="B2">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="C2">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="D2">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="E2">
-        <v>87</v>
+        <v>44</v>
       </c>
       <c r="F2">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="G2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="H2">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="I2">
-        <v>79</v>
+        <v>14</v>
       </c>
       <c r="J2">
-        <v>6</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>992189</v>
+        <v>99882</v>
       </c>
       <c r="B3">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="C3">
+        <v>75</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>38</v>
+      </c>
+      <c r="F3">
         <v>19</v>
       </c>
-      <c r="D3">
-        <v>62</v>
-      </c>
-      <c r="E3">
-        <v>92</v>
-      </c>
-      <c r="F3">
-        <v>69</v>
-      </c>
       <c r="G3">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="H3">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="I3">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J3">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>992119</v>
+        <v>99883</v>
       </c>
       <c r="B4">
         <v>49</v>
       </c>
       <c r="C4">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="D4">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="E4">
+        <v>66</v>
+      </c>
+      <c r="F4">
         <v>94</v>
       </c>
-      <c r="F4">
-        <v>62</v>
-      </c>
       <c r="G4">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="H4">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="I4">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="J4">
-        <v>88</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>992139</v>
+        <v>99884</v>
       </c>
       <c r="B5">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C5">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="D5">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="F5">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="G5">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="I5">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="J5">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>992129</v>
-      </c>
-      <c r="B6">
-        <v>40</v>
-      </c>
-      <c r="C6">
-        <v>72</v>
-      </c>
-      <c r="D6">
-        <v>52</v>
-      </c>
-      <c r="E6">
-        <v>58</v>
-      </c>
-      <c r="F6">
-        <v>50</v>
-      </c>
-      <c r="G6">
-        <v>81</v>
-      </c>
-      <c r="H6">
-        <v>70</v>
-      </c>
-      <c r="I6">
-        <v>50</v>
-      </c>
-      <c r="J6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>992149</v>
-      </c>
-      <c r="B7">
-        <v>33</v>
-      </c>
-      <c r="C7">
-        <v>63</v>
-      </c>
-      <c r="D7">
-        <v>50</v>
-      </c>
-      <c r="E7">
-        <v>74</v>
-      </c>
-      <c r="F7">
-        <v>63</v>
-      </c>
-      <c r="G7">
-        <v>72</v>
-      </c>
-      <c r="H7">
-        <v>23</v>
-      </c>
-      <c r="I7">
-        <v>59</v>
-      </c>
-      <c r="J7">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>992159</v>
-      </c>
-      <c r="B8">
-        <v>65</v>
-      </c>
-      <c r="C8">
-        <v>100</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>82</v>
-      </c>
-      <c r="F8">
-        <v>52</v>
-      </c>
-      <c r="G8">
-        <v>26</v>
-      </c>
-      <c r="H8">
-        <v>70</v>
-      </c>
-      <c r="I8">
-        <v>81</v>
-      </c>
-      <c r="J8">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>992169</v>
-      </c>
-      <c r="B9">
-        <v>81</v>
-      </c>
-      <c r="C9">
-        <v>50</v>
-      </c>
-      <c r="D9">
         <v>69</v>
-      </c>
-      <c r="E9">
-        <v>56</v>
-      </c>
-      <c r="F9">
-        <v>44</v>
-      </c>
-      <c r="G9">
-        <v>32</v>
-      </c>
-      <c r="H9">
-        <v>20</v>
-      </c>
-      <c r="I9">
-        <v>60</v>
-      </c>
-      <c r="J9">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>